<commit_message>
add link to coverage in counters vplan
Signed-off-by: Robin Pedersen <Robin.Pedersen@silabs.com>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/Simulation/privileged_spec/CV32E40X_Counters.xlsx
+++ b/docs/VerifPlans/Simulation/privileged_spec/CV32E40X_Counters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\counters_vplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71BF789-0921-478E-903E-7B26C669A644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3740E1-6642-42F3-8BB0-1D243EAB0791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="127">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -448,6 +448,21 @@
   </si>
   <si>
     <t>Updating retirement-related counters must have happened within the time the instruction is considered retired (i.e. must be visible on the rvfi retirement)</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_check_mcycle</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_check_minstret</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.cg_idx_wrapper_*.mhpm_cg.x_check_mhpm</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.cg_idx_wrapper_*.inhibit_mix_cg.x_check_*</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_minstret_in_dbg</t>
   </si>
 </sst>
 </file>
@@ -580,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -642,6 +657,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,27 +1073,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="72" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="54.5703125" style="1" customWidth="1"/>
     <col min="11" max="1024" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="45">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1104,14 +1125,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1129,13 +1150,15 @@
       <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="24" t="s">
+        <v>122</v>
+      </c>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="24"/>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="8" t="s">
         <v>57</v>
       </c>
@@ -1151,13 +1174,15 @@
       <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15"/>
+      <c r="I3" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="13" t="s">
         <v>70</v>
       </c>
@@ -1173,13 +1198,15 @@
       <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="23" t="s">
+        <v>124</v>
+      </c>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="24"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="14" t="s">
         <v>112</v>
       </c>
@@ -1195,16 +1222,18 @@
       <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="23" t="s">
+        <v>125</v>
+      </c>
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="24" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="28" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -1219,14 +1248,16 @@
       <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="24" t="s">
+        <v>122</v>
+      </c>
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="10" t="s">
         <v>55</v>
       </c>
@@ -1239,16 +1270,16 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -1263,14 +1294,16 @@
       <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="26"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14" t="s">
         <v>117</v>
       </c>
@@ -1283,12 +1316,12 @@
       <c r="H9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="165">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
@@ -1313,12 +1346,12 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="27" t="s">
         <v>118</v>
       </c>
       <c r="E11" s="14" t="s">
@@ -1337,10 +1370,10 @@
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="14" t="s">
         <v>74</v>
       </c>
@@ -1357,10 +1390,10 @@
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="90">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -1387,8 +1420,8 @@
       <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="18" t="s">
         <v>76</v>
       </c>
@@ -1411,8 +1444,8 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="18" t="s">
         <v>37</v>
       </c>
@@ -1435,8 +1468,8 @@
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="18" t="s">
         <v>31</v>
       </c>
@@ -1459,8 +1492,8 @@
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="18" t="s">
         <v>33</v>
       </c>
@@ -1483,8 +1516,8 @@
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="18" t="s">
         <v>35</v>
       </c>
@@ -1507,8 +1540,8 @@
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="18" t="s">
         <v>77</v>
       </c>
@@ -1531,8 +1564,8 @@
       <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="18" t="s">
         <v>78</v>
       </c>
@@ -1555,8 +1588,8 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="18" t="s">
         <v>79</v>
       </c>
@@ -1579,8 +1612,8 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="18" t="s">
         <v>80</v>
       </c>
@@ -1603,8 +1636,8 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="18" t="s">
         <v>81</v>
       </c>
@@ -1627,8 +1660,8 @@
       <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="18" t="s">
         <v>85</v>
       </c>
@@ -1651,8 +1684,8 @@
       <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="18" t="s">
         <v>86</v>
       </c>
@@ -1675,8 +1708,8 @@
       <c r="J25" s="12"/>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="18" t="s">
         <v>87</v>
       </c>
@@ -1699,8 +1732,8 @@
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="18" t="s">
         <v>90</v>
       </c>
@@ -1723,8 +1756,8 @@
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="18" t="s">
         <v>96</v>
       </c>
@@ -1747,8 +1780,8 @@
       <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="18" t="s">
         <v>110</v>
       </c>
@@ -1771,8 +1804,8 @@
       <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="60">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="19" t="s">
         <v>114</v>
       </c>
@@ -1795,16 +1828,16 @@
       <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="32" t="s">
         <v>64</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -1823,10 +1856,10 @@
       <c r="J31" s="12"/>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A32" s="26"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="12" t="s">
         <v>66</v>
       </c>
@@ -1839,16 +1872,18 @@
       <c r="H32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J32" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A33" s="26"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="12" t="s">
         <v>68</v>
       </c>
@@ -1889,18 +1924,18 @@
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" s="5" customFormat="1">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
Merge from upstream cv32e40x/dev
Signed-off-by: Robin Pedersen <Robin.Pedersen@silabs.com>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/Simulation/privileged_spec/CV32E40X_Counters.xlsx
+++ b/docs/VerifPlans/Simulation/privileged_spec/CV32E40X_Counters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\counters_vplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71BF789-0921-478E-903E-7B26C669A644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3740E1-6642-42F3-8BB0-1D243EAB0791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="127">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -448,6 +448,21 @@
   </si>
   <si>
     <t>Updating retirement-related counters must have happened within the time the instruction is considered retired (i.e. must be visible on the rvfi retirement)</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_check_mcycle</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_check_minstret</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.cg_idx_wrapper_*.mhpm_cg.x_check_mhpm</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.cg_idx_wrapper_*.inhibit_mix_cg.x_check_*</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_minstret_in_dbg</t>
   </si>
 </sst>
 </file>
@@ -580,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -642,6 +657,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,27 +1073,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="72" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="54.5703125" style="1" customWidth="1"/>
     <col min="11" max="1024" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="45">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1104,14 +1125,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1129,13 +1150,15 @@
       <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="24" t="s">
+        <v>122</v>
+      </c>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="24"/>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="8" t="s">
         <v>57</v>
       </c>
@@ -1151,13 +1174,15 @@
       <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15"/>
+      <c r="I3" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="13" t="s">
         <v>70</v>
       </c>
@@ -1173,13 +1198,15 @@
       <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="23" t="s">
+        <v>124</v>
+      </c>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="24"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="14" t="s">
         <v>112</v>
       </c>
@@ -1195,16 +1222,18 @@
       <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="23" t="s">
+        <v>125</v>
+      </c>
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="24" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="28" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="17" t="s">
@@ -1219,14 +1248,16 @@
       <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="24" t="s">
+        <v>122</v>
+      </c>
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="10" t="s">
         <v>55</v>
       </c>
@@ -1239,16 +1270,16 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -1263,14 +1294,16 @@
       <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="26"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="14" t="s">
         <v>117</v>
       </c>
@@ -1283,12 +1316,12 @@
       <c r="H9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="165">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
@@ -1313,12 +1346,12 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="27" t="s">
         <v>118</v>
       </c>
       <c r="E11" s="14" t="s">
@@ -1337,10 +1370,10 @@
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="14" t="s">
         <v>74</v>
       </c>
@@ -1357,10 +1390,10 @@
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="90">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -1387,8 +1420,8 @@
       <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="18" t="s">
         <v>76</v>
       </c>
@@ -1411,8 +1444,8 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="18" t="s">
         <v>37</v>
       </c>
@@ -1435,8 +1468,8 @@
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="18" t="s">
         <v>31</v>
       </c>
@@ -1459,8 +1492,8 @@
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="18" t="s">
         <v>33</v>
       </c>
@@ -1483,8 +1516,8 @@
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="18" t="s">
         <v>35</v>
       </c>
@@ -1507,8 +1540,8 @@
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="18" t="s">
         <v>77</v>
       </c>
@@ -1531,8 +1564,8 @@
       <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="18" t="s">
         <v>78</v>
       </c>
@@ -1555,8 +1588,8 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="18" t="s">
         <v>79</v>
       </c>
@@ -1579,8 +1612,8 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="18" t="s">
         <v>80</v>
       </c>
@@ -1603,8 +1636,8 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="18" t="s">
         <v>81</v>
       </c>
@@ -1627,8 +1660,8 @@
       <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="18" t="s">
         <v>85</v>
       </c>
@@ -1651,8 +1684,8 @@
       <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="18" t="s">
         <v>86</v>
       </c>
@@ -1675,8 +1708,8 @@
       <c r="J25" s="12"/>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="18" t="s">
         <v>87</v>
       </c>
@@ -1699,8 +1732,8 @@
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="18" t="s">
         <v>90</v>
       </c>
@@ -1723,8 +1756,8 @@
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="18" t="s">
         <v>96</v>
       </c>
@@ -1747,8 +1780,8 @@
       <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="18" t="s">
         <v>110</v>
       </c>
@@ -1771,8 +1804,8 @@
       <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="60">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="19" t="s">
         <v>114</v>
       </c>
@@ -1795,16 +1828,16 @@
       <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="32" t="s">
         <v>64</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -1823,10 +1856,10 @@
       <c r="J31" s="12"/>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="45">
-      <c r="A32" s="26"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="12" t="s">
         <v>66</v>
       </c>
@@ -1839,16 +1872,18 @@
       <c r="H32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J32" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" ht="30">
-      <c r="A33" s="26"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="12" t="s">
         <v>68</v>
       </c>
@@ -1889,18 +1924,18 @@
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" s="5" customFormat="1">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
Add link to coverage for minstret test
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/Simulation/privileged_spec/CV32E40X_Counters.xlsx
+++ b/docs/VerifPlans/Simulation/privileged_spec/CV32E40X_Counters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF64077-DFEB-46F2-A110-9440EE4E154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33611EC5-9C8F-45F9-A137-B6E8A83A1DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25095" yWindow="16080" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CV32E40X Counters" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="129">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -466,6 +466,9 @@
   </si>
   <si>
     <t>mcycle continues during debug if stopcount=0, and stop if stopcount=1</t>
+  </si>
+  <si>
+    <t>uvm_pkg.uvm_test_top.env.cov_model.counters_covg.counters_cg.x_check_minstret. RTC: corev_rand_arithmetic_base_test CFG=enable_counters_std , corev_rand_instr_test CFG=enable_counters_std</t>
   </si>
 </sst>
 </file>
@@ -1060,9 +1063,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -1260,7 +1263,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:10" customFormat="1" ht="42.75">
+    <row r="8" spans="1:10" customFormat="1" ht="99.75">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
       <c r="C8" s="22" t="s">
@@ -1282,7 +1285,7 @@
         <v>20</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="J8" s="19"/>
     </row>

</xml_diff>